<commit_message>
mas 12 4 2021
</commit_message>
<xml_diff>
--- a/Account.xlsx
+++ b/Account.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="52">
   <si>
     <t xml:space="preserve">Pias vai </t>
   </si>
@@ -157,6 +157,21 @@
   </si>
   <si>
     <t>Oil</t>
+  </si>
+  <si>
+    <t>Mas+ Peaj +roshun+riska</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shim </t>
+  </si>
+  <si>
+    <t>kopi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">peaj pata </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mas </t>
   </si>
 </sst>
 </file>
@@ -501,7 +516,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -568,6 +583,52 @@
         <v>55</v>
       </c>
     </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4">
+        <v>750</v>
+      </c>
+      <c r="E4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8">
+        <v>110</v>
+      </c>
+    </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20">
         <f>SUM(B2:B19)</f>
@@ -575,17 +636,17 @@
       </c>
       <c r="D20">
         <f>SUM(D2:D19)</f>
-        <v>200</v>
+        <v>950</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22">
         <f>SUM(D25-B20)</f>
-        <v>-115</v>
+        <v>205</v>
       </c>
       <c r="D22">
         <f>SUM(D25-D20)</f>
-        <v>5</v>
+        <v>-425</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
@@ -594,11 +655,11 @@
       </c>
       <c r="D24">
         <f>SUM(D20,F24,B20)</f>
-        <v>615</v>
+        <v>1575</v>
       </c>
       <c r="F24">
         <f>SUM(F2:F23)</f>
-        <v>95</v>
+        <v>305</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
@@ -607,13 +668,13 @@
       </c>
       <c r="D25">
         <f>D24/3</f>
-        <v>205</v>
+        <v>525</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F26">
         <f>SUM(D25-F24)</f>
-        <v>110</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
12 6 21 rich mosla
</commit_message>
<xml_diff>
--- a/Account.xlsx
+++ b/Account.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="57">
   <si>
     <t xml:space="preserve">Pias vai </t>
   </si>
@@ -172,6 +172,21 @@
   </si>
   <si>
     <t xml:space="preserve">Mas </t>
+  </si>
+  <si>
+    <t>2kg alu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">holud gura + Jira gura </t>
+  </si>
+  <si>
+    <t xml:space="preserve">shak </t>
+  </si>
+  <si>
+    <t>Chal</t>
+  </si>
+  <si>
+    <t>Rishka</t>
   </si>
 </sst>
 </file>
@@ -516,7 +531,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -629,6 +644,46 @@
         <v>110</v>
       </c>
     </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13">
+        <v>20</v>
+      </c>
+    </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20">
         <f>SUM(B2:B19)</f>
@@ -642,11 +697,11 @@
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22">
         <f>SUM(D25-B20)</f>
-        <v>205</v>
+        <v>358.33333333333337</v>
       </c>
       <c r="D22">
         <f>SUM(D25-D20)</f>
-        <v>-425</v>
+        <v>-271.66666666666663</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
@@ -655,11 +710,11 @@
       </c>
       <c r="D24">
         <f>SUM(D20,F24,B20)</f>
-        <v>1575</v>
+        <v>2035</v>
       </c>
       <c r="F24">
         <f>SUM(F2:F23)</f>
-        <v>305</v>
+        <v>765</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
@@ -668,13 +723,13 @@
       </c>
       <c r="D25">
         <f>D24/3</f>
-        <v>525</v>
+        <v>678.33333333333337</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F26">
         <f>SUM(D25-F24)</f>
-        <v>220</v>
+        <v>-86.666666666666629</v>
       </c>
     </row>
   </sheetData>

</xml_diff>